<commit_message>
fix fe image input
</commit_message>
<xml_diff>
--- a/output/train_experiments_results.xlsx
+++ b/output/train_experiments_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdal\Documents\Master\EMJMD MAIA\SEMESTER 3 - UdG\CAD\Melanoma-classification-using-machine-learning\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A99F83-6A58-492E-98AE-A3B6F5C8099E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE57EF6-2ABB-4C04-B560-9494D72A18CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Experiment Count</t>
   </si>
@@ -33,40 +33,49 @@
     <t>Features</t>
   </si>
   <si>
+    <t>N_Features</t>
+  </si>
+  <si>
+    <t>1000 / class</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Feature Selection</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Data Shuffled</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Best Model</t>
+  </si>
+  <si>
+    <t>SVC(C=1000, gamma=0.001)</t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>37m 45.8s</t>
+  </si>
+  <si>
     <t>Color (RGB) + GLCM</t>
   </si>
   <si>
-    <t>N_Features</t>
-  </si>
-  <si>
-    <t>1000 / class</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Feature Selection</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Data Shuffled</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Best Model</t>
-  </si>
-  <si>
-    <t>SVC(C=1000, gamma=0.001)</t>
-  </si>
-  <si>
-    <t>Training Time</t>
-  </si>
-  <si>
-    <t>37m 45.8s</t>
+    <t>1000/ class</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>48m 34.6s</t>
   </si>
 </sst>
 </file>
@@ -156,17 +165,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B2:I3" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I5" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,7 +447,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,22 +470,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -488,25 +497,25 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
         <v>0.74324324324324298</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -514,14 +523,30 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.74274274274274199</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>

</xml_diff>

<commit_message>
added lbp and hsv features, retrain sample
</commit_message>
<xml_diff>
--- a/output/train_experiments_results.xlsx
+++ b/output/train_experiments_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdal\Documents\Master\EMJMD MAIA\SEMESTER 3 - UdG\CAD\Melanoma-classification-using-machine-learning\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE57EF6-2ABB-4C04-B560-9494D72A18CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96613B81-2D19-4F20-9AFE-3F33CC950745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Experiment Count</t>
   </si>
@@ -69,13 +69,19 @@
     <t>Color (RGB) + GLCM</t>
   </si>
   <si>
-    <t>1000/ class</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>48m 34.6s</t>
+  </si>
+  <si>
+    <t>Color (RGB + HSV) + GLCM + LBP</t>
+  </si>
+  <si>
+    <t>SVC(C=100, gamma=0.001)</t>
+  </si>
+  <si>
+    <t>146m 59.5s</t>
   </si>
 </sst>
 </file>
@@ -447,13 +453,13 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.08984375" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="22.54296875" customWidth="1"/>
     <col min="6" max="6" width="18.81640625" customWidth="1"/>
@@ -530,10 +536,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -545,7 +551,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -553,14 +559,30 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.79729729729729704</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>

</xml_diff>

<commit_message>
train all models on all features and save experiment results
</commit_message>
<xml_diff>
--- a/output/train_experiments_results.xlsx
+++ b/output/train_experiments_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdal\Documents\Master\EMJMD MAIA\SEMESTER 3 - UdG\CAD\Melanoma-classification-using-machine-learning\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96613B81-2D19-4F20-9AFE-3F33CC950745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC8A7AE-B9DC-4D77-A9F5-D579B1AB0F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Experiment Count</t>
   </si>
@@ -82,13 +82,70 @@
   </si>
   <si>
     <t>146m 59.5s</t>
+  </si>
+  <si>
+    <t>All Features</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Best Pramars</t>
+  </si>
+  <si>
+    <t>SVC(C=10, gamma=0.01)</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.01, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>XGBClassifier</t>
+  </si>
+  <si>
+    <t>{'colsample_bytree': 1.0, 'learning_rate': 0.1, 'max_depth': 5, 'n_estimators': 300, 'subsample': 0.7}</t>
+  </si>
+  <si>
+    <t>KNeighborsClassifier</t>
+  </si>
+  <si>
+    <t>{'algorithm': 'ball_tree', 'n_neighbors': 9, 'p': 2, 'weights': 'distance'}</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier</t>
+  </si>
+  <si>
+    <t>{'max_depth': 9, 'min_samples_leaf': 4, 'min_samples_split': 2, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>LogisticRegression</t>
+  </si>
+  <si>
+    <t>{'C': 0.1, 'penalty': None, 'solver': 'newton-cholesky'}</t>
+  </si>
+  <si>
+    <t>LinearDiscriminantAnalysis</t>
+  </si>
+  <si>
+    <t>{'shrinkage': None, 'solver': 'svd'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,19 +153,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -117,16 +241,350 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -171,17 +629,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I5" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}" name="Table1" displayName="Table1" ref="B2:I6" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B2:I6" xr:uid="{71817D4A-3D4C-4F66-A734-34681A6B3F8D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{54EAE10A-532E-4BB1-B31F-24D329163B33}" name="Experiment Count" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{7F3B76A9-D3E2-448F-97D5-27D070AD936F}" name="Features" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{640C8F46-26F7-4737-8FD4-3681257719C1}" name="N_Features" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{829793FC-5371-4E06-857A-E81C01DCC6B7}" name="Data Shuffled" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{FDA46974-FD10-4FE3-86E9-3738008ACD61}" name="Feature Selection" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{1A2A58B8-007C-4EE4-968F-7E1F4AD953AD}" name="Accuracy" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{DE8EA16D-260C-4201-A42F-201C975EAC9E}" name="Best Model" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{0D4A10FD-63CF-4EE8-811F-4A013EEE3077}" name="Training Time" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}" name="Table2" displayName="Table2" ref="B13:M19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="14">
+  <autoFilter ref="B13:M19" xr:uid="{203D055E-7DCE-4ECB-ADB4-FA1FA74C4F29}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{B1948067-CB65-4206-AE71-0D57640D7089}" name="Experiment Count" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{FDDCB198-EAE1-4ED4-A066-F8DBAC98C717}" name="Features" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{83D1AD7E-916A-4241-B599-9349DCDB2027}" name="N_Features" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{70DAF01F-DAE6-4B77-9BDB-7F5053A6F854}" name="Data Shuffled" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{3B5E59E9-2BF5-4D6D-816E-23251AFDB13E}" name="Feature Selection" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{F7473F45-1D6D-409F-9883-1FD36FD545E3}" name="Model" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{90C55BBC-BCBC-4A00-8864-5A767EA01E45}" name="Accuracy" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{75867AB3-1849-4FCA-B58F-BE8AEF3B207D}" name="F1" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{B2F22562-6078-45C9-A5D5-49F1FBF2A4F1}" name="Sensitivity" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{72664E3E-D59C-4D9C-8541-496AB288C8B6}" name="Specificity" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{0FEE43E7-8EFC-4D86-86B0-C5FE824F8CBB}" name="Precision" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C971C848-AE17-4A17-898B-01154D7A5111}" name="Best Pramars" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -453,7 +932,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,9 +942,13 @@
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="22.54296875" customWidth="1"/>
     <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
     <col min="8" max="8" width="26.6328125" customWidth="1"/>
     <col min="9" max="9" width="23.26953125" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6328125" customWidth="1"/>
+    <col min="12" max="12" width="20.90625" customWidth="1"/>
+    <col min="13" max="13" width="83.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
@@ -687,108 +1170,277 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.81401475237091603</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.81193393713372297</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.81715817694369897</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.81097876747799003</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.80677607199576495</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.80400421496311902</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.80149413020277405</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.80536193029490599</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0.80269290523045</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.79766330323951096</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.78503688092729096</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.78694516971279305</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.80804289544235897</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.76281719316416297</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.76692111959287501</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="B17" s="6">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.78055848261327698</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.77968791325046205</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.79034852546916801</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.77110305541170299</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.76931106471816202</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.77660695468914598</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0.77167474421109294</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.76836461126005295</v>
+      </c>
+      <c r="K18" s="8">
+        <v>0.78456758156395601</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.77501352082206598</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="B19" s="6">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.77634351949420399</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.77134392674387298</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.76782841823056303</v>
+      </c>
+      <c r="K19" s="8">
+        <v>0.78456758156395601</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.77489177489177397</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>